<commit_message>
updated for EXPLORE behavior
</commit_message>
<xml_diff>
--- a/SuppleLookupTable.xlsx
+++ b/SuppleLookupTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dombrovski\Desktop\EXPLORE\explore_clock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DNPL\Documents\GitHub\explore_clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C02449-C906-4877-86FC-3E8DEAC40168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="14310"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Control</t>
   </si>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,6 +170,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -204,6 +222,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -379,22 +414,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A51"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -422,318 +457,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -742,24 +473,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>